<commit_message>
them chuc nang : 1. them thong tin benh nhan tu ben thu 3 2. tao api cho ben thu 3 print ticket 3.
</commit_message>
<xml_diff>
--- a/GPRO_QMS_Web/Report Template/Report QMS Template.xlsx
+++ b/GPRO_QMS_Web/Report Template/Report QMS Template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,12 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -135,6 +132,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -289,7 +292,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,7 +327,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -533,86 +536,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="5" t="s">
+    <row r="1" spans="1:14" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="2:14" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="5" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="D5"/>
       <c r="E5"/>
@@ -620,7 +630,7 @@
       <c r="G5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="D6"/>
       <c r="E6"/>
@@ -628,7 +638,7 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="D7"/>
       <c r="E7"/>
@@ -636,7 +646,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="D8"/>
       <c r="E8"/>
@@ -644,7 +654,7 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="D9"/>
       <c r="E9"/>
@@ -652,7 +662,7 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="D10"/>
       <c r="E10"/>
@@ -660,7 +670,7 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="D11"/>
       <c r="E11"/>
@@ -668,7 +678,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="D12"/>
       <c r="E12"/>
@@ -676,7 +686,7 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="D13"/>
       <c r="E13"/>
@@ -684,7 +694,7 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="D14"/>
       <c r="E14"/>
@@ -692,7 +702,7 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="D15"/>
       <c r="E15"/>
@@ -700,7 +710,7 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="D16"/>
       <c r="E16"/>
@@ -708,7 +718,7 @@
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="D17"/>
       <c r="E17"/>
@@ -716,7 +726,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="D18"/>
       <c r="E18"/>
@@ -724,7 +734,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="D19"/>
       <c r="E19"/>
@@ -732,7 +742,7 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="D20"/>
       <c r="E20"/>
@@ -740,7 +750,7 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="D21"/>
       <c r="E21"/>
@@ -748,7 +758,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="D22"/>
       <c r="E22"/>
@@ -756,7 +766,7 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="D23"/>
       <c r="E23"/>
@@ -764,7 +774,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="D24"/>
       <c r="E24"/>
@@ -772,7 +782,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="D25"/>
       <c r="E25"/>
@@ -780,7 +790,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="D26"/>
       <c r="E26"/>
@@ -788,7 +798,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="D27"/>
       <c r="E27"/>
@@ -796,7 +806,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="D28"/>
       <c r="E28"/>
@@ -804,7 +814,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="D29"/>
       <c r="E29"/>
@@ -812,7 +822,7 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="D30"/>
       <c r="E30"/>
@@ -820,7 +830,7 @@
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="D31"/>
       <c r="E31"/>
@@ -828,7 +838,7 @@
       <c r="G31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="D32"/>
       <c r="E32"/>
@@ -836,7 +846,7 @@
       <c r="G32"/>
       <c r="H32"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="D33"/>
       <c r="E33"/>
@@ -844,7 +854,7 @@
       <c r="G33"/>
       <c r="H33"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="D34"/>
       <c r="E34"/>
@@ -852,7 +862,7 @@
       <c r="G34"/>
       <c r="H34"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="D35"/>
       <c r="E35"/>
@@ -860,7 +870,7 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="D36"/>
       <c r="E36"/>
@@ -868,7 +878,7 @@
       <c r="G36"/>
       <c r="H36"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="D37"/>
       <c r="E37"/>
@@ -876,7 +886,7 @@
       <c r="G37"/>
       <c r="H37"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="D38"/>
       <c r="E38"/>
@@ -884,7 +894,7 @@
       <c r="G38"/>
       <c r="H38"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="D39"/>
       <c r="E39"/>
@@ -892,7 +902,7 @@
       <c r="G39"/>
       <c r="H39"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="D40"/>
       <c r="E40"/>
@@ -900,7 +910,7 @@
       <c r="G40"/>
       <c r="H40"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="D41"/>
       <c r="E41"/>
@@ -908,7 +918,7 @@
       <c r="G41"/>
       <c r="H41"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="D42"/>
       <c r="E42"/>
@@ -916,7 +926,7 @@
       <c r="G42"/>
       <c r="H42"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="D43"/>
       <c r="E43"/>
@@ -924,7 +934,7 @@
       <c r="G43"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="D44"/>
       <c r="E44"/>
@@ -932,7 +942,7 @@
       <c r="G44"/>
       <c r="H44"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="D45"/>
       <c r="E45"/>
@@ -940,7 +950,7 @@
       <c r="G45"/>
       <c r="H45"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="D46"/>
       <c r="E46"/>
@@ -948,7 +958,7 @@
       <c r="G46"/>
       <c r="H46"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="D47"/>
       <c r="E47"/>
@@ -956,7 +966,7 @@
       <c r="G47"/>
       <c r="H47"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="D48"/>
       <c r="E48"/>
@@ -964,7 +974,7 @@
       <c r="G48"/>
       <c r="H48"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="D49"/>
       <c r="E49"/>
@@ -972,7 +982,7 @@
       <c r="G49"/>
       <c r="H49"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="D50"/>
       <c r="E50"/>
@@ -980,7 +990,7 @@
       <c r="G50"/>
       <c r="H50"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="D51"/>
       <c r="E51"/>
@@ -995,7 +1005,7 @@
     <mergeCell ref="B3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>